<commit_message>
adding date formating action that format a date column to a specific format
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/SortExcel/test_data.xlsx
+++ b/src/test/resources/test_files/SortExcel/test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
   <si>
     <t>Apple</t>
   </si>
@@ -53,8 +53,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -85,12 +86,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -493,7 +503,7 @@
       <c r="B2" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C2" t="n" s="2">
+      <c r="C2" t="n" s="11">
         <v>44691.0</v>
       </c>
       <c r="D2" t="s" s="0">
@@ -507,7 +517,7 @@
       <c r="B3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C3" t="n" s="3">
+      <c r="C3" t="n" s="12">
         <v>44531.0</v>
       </c>
       <c r="D3" t="s" s="0">
@@ -521,7 +531,7 @@
       <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C4" t="n" s="4">
+      <c r="C4" t="n" s="13">
         <v>44941.0</v>
       </c>
       <c r="D4" t="s" s="0">

</xml_diff>

<commit_message>
adding comments to make the code more readable and understandable by colleagues
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/SortExcel/test_data.xlsx
+++ b/src/test/resources/test_files/SortExcel/test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="11">
   <si>
     <t>Apple</t>
   </si>
@@ -86,7 +86,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -98,6 +98,12 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -503,7 +509,7 @@
       <c r="B2" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C2" t="n" s="11">
+      <c r="C2" t="n" s="17">
         <v>44691.0</v>
       </c>
       <c r="D2" t="s" s="0">
@@ -517,7 +523,7 @@
       <c r="B3" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="C3" t="n" s="12">
+      <c r="C3" t="n" s="18">
         <v>44531.0</v>
       </c>
       <c r="D3" t="s" s="0">
@@ -531,7 +537,7 @@
       <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="C4" t="n" s="13">
+      <c r="C4" t="n" s="19">
         <v>44941.0</v>
       </c>
       <c r="D4" t="s" s="0">

</xml_diff>